<commit_message>
Added CommonDataProvider to run multiple @Test with same dataprovider
</commit_message>
<xml_diff>
--- a/test-data/orange-hrm-data.xlsx
+++ b/test-data/orange-hrm-data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SessionWork\HybridFramework\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0722CD4B-1B24-4152-BC40-243925F5A7B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BBE0B9-46C3-45DA-8F2B-3D32AE978C81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" activeTab="1" xr2:uid="{2D4BB6AE-0877-4019-841D-C410490929AC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" activeTab="3" xr2:uid="{2D4BB6AE-0877-4019-841D-C410490929AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="invalidLoginTest" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="validLoginTest" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -43,9 +44,6 @@
     <t>Invalid credentials</t>
   </si>
   <si>
-    <t>john</t>
-  </si>
-  <si>
     <t>john123</t>
   </si>
   <si>
@@ -62,6 +60,12 @@
   </si>
   <si>
     <t>Quick Launch</t>
+  </si>
+  <si>
+    <t>saul</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -425,10 +429,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6611FA3C-843D-4DA8-B000-1DFB4B1CBE0E}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,10 +455,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -465,9 +469,20 @@
         <v>455</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -490,10 +505,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1285D50E-6893-47A4-B71E-68EEB0884594}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,18 +524,29 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -529,6 +555,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB07F6A-D072-4602-82BB-9B414533CDF4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92533907-5B9C-4977-A410-BFAACA207DC0}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>